<commit_message>
**Untested Commit before Dallas** Added 'wait on xxx FAST' commands
Added conditional variable "CMD_TYPE" which can be SAFE or FAST
</commit_message>
<xml_diff>
--- a/Competition Code/Auton Tests.xlsx
+++ b/Competition Code/Auton Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="13515" windowHeight="1815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>Recommended Setting</t>
   </si>
   <si>
-    <t>Slight overshoot, not 'exact' but should be good enough</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>GYRO_DRIVE_STRAIGHT 60 0.65</t>
   </si>
   <si>
-    <t>Doesn’t correct at first or for small distances</t>
-  </si>
-  <si>
     <t>GYRO_STRAFE_STRAIGHT</t>
   </si>
   <si>
@@ -136,14 +130,54 @@
   </si>
   <si>
     <t>GYRO_DRIVE_STRAIGHT **FOR OVER THE RAMP settings***</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Doesn’t correct at first or for small distances - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NEGATIVE IS LEFT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Slight overshoot, not 'exact' but should be good enough - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NEGATIVE IS LEFT</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -476,14 +510,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
     <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -506,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -514,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -522,7 +556,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,7 +564,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -538,13 +572,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -552,13 +586,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -572,7 +606,7 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -580,7 +614,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -596,35 +630,35 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -652,7 +686,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -690,11 +724,12 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changes from Thursday at Hub City
1. Sensor filter broke on L gripper, changed the PID constant on that motor to accommodate. Problem is still an overshoot, which is bad for the 'RC' position because it can overshoot past the rollover point. Long term solution would be to either fix the filter or move the rollover point again

2. Changed cycle button action to go to 1 since we are trying to pick up 2 totes
</commit_message>
<xml_diff>
--- a/Competition Code/Auton Tests.xlsx
+++ b/Competition Code/Auton Tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>TANK_DRIVE_TIME &lt;LEFT&gt; &lt;RIGHT&gt; &lt;TIME (s)&gt;</t>
   </si>
@@ -168,7 +168,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +181,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -202,13 +212,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -510,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,21 +678,33 @@
       <c r="A14" t="s">
         <v>9</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -693,30 +718,48 @@
       <c r="A19" t="s">
         <v>14</v>
       </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>